<commit_message>
New questions + Custom result page update
</commit_message>
<xml_diff>
--- a/Covid19Quiz.xlsx
+++ b/Covid19Quiz.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rohitchoudhary/perpro/corona-quiz/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{131989D9-67CB-6146-A1E2-978780158C58}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38D12D54-54D4-9440-A5BC-B9B8A5F7BD26}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="123">
   <si>
     <t>question</t>
   </si>
@@ -306,6 +306,90 @@
   <si>
     <t>Covid-19 can be transmitted in hot and humid areas.</t>
   </si>
+  <si>
+    <t>Can I catch the coronavirus disease (COVID-19) from my pet?</t>
+  </si>
+  <si>
+    <t>The Coronavirus can be transmitted through mosquito bites.</t>
+  </si>
+  <si>
+    <t>Are hand dryers effective in killing the new coronavirus?</t>
+  </si>
+  <si>
+    <t>Can you catch the Coronavirus and show no symptoms?</t>
+  </si>
+  <si>
+    <t>Yes, because it has 5 days incubation period</t>
+  </si>
+  <si>
+    <t>No, symptoms are visible from day 1</t>
+  </si>
+  <si>
+    <t>Can you catch the Coronavirus for the second time?</t>
+  </si>
+  <si>
+    <t>You can get infected again</t>
+  </si>
+  <si>
+    <t>You only get infected once</t>
+  </si>
+  <si>
+    <t>Depends on how long the immunity of the patient lasts</t>
+  </si>
+  <si>
+    <t>How long can the Cornonavirus survive on surfaces?</t>
+  </si>
+  <si>
+    <t>It doesn't stick to surfaces</t>
+  </si>
+  <si>
+    <t>Surfaces remain infected always</t>
+  </si>
+  <si>
+    <t>Depends on the surface material and the amount of virus present</t>
+  </si>
+  <si>
+    <t>How long can the Cornonavirus survive on copper?</t>
+  </si>
+  <si>
+    <t>Up to 5hrs</t>
+  </si>
+  <si>
+    <t>Up to 4hrs</t>
+  </si>
+  <si>
+    <t>Up to 3hrs</t>
+  </si>
+  <si>
+    <t>How long can the Cornonavirus survive on cardboard?</t>
+  </si>
+  <si>
+    <t>Up to 24hrs</t>
+  </si>
+  <si>
+    <t>Up to 20hrs</t>
+  </si>
+  <si>
+    <t>Up to 15hrs</t>
+  </si>
+  <si>
+    <t>How long can the Cornonavirus survive on plastic?</t>
+  </si>
+  <si>
+    <t>Up to 3 days</t>
+  </si>
+  <si>
+    <t>Up to 5 days</t>
+  </si>
+  <si>
+    <t>Up to 7 days</t>
+  </si>
+  <si>
+    <t>How long can the Cornonavirus survive on stainless steel?</t>
+  </si>
+  <si>
+    <t>How long can the Cornonavirus survive in air?</t>
+  </si>
 </sst>
 </file>
 
@@ -568,7 +652,7 @@
   <dimension ref="A1:Y998"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection sqref="A1:M24"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1359,25 +1443,24 @@
       <c r="D17" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1">
+      <c r="E17" s="1">
         <v>3</v>
       </c>
-      <c r="G17" s="1" t="s">
+      <c r="F17" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="I17" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K17" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="L17" s="1"/>
-      <c r="M17" s="1">
+      <c r="K17" s="1"/>
+      <c r="L17" s="1">
         <v>10</v>
       </c>
       <c r="N17" s="1"/>
@@ -1723,19 +1806,39 @@
       <c r="Y24" s="1"/>
     </row>
     <row r="25" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
+      <c r="A25" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>70</v>
+      </c>
       <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
+      <c r="F25" s="1">
+        <v>2</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="H25" s="1"/>
-      <c r="I25" s="1"/>
-      <c r="J25" s="1"/>
-      <c r="K25" s="1"/>
+      <c r="I25" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="L25" s="1"/>
-      <c r="M25" s="1"/>
+      <c r="M25" s="1">
+        <v>10</v>
+      </c>
       <c r="N25" s="1"/>
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
@@ -1750,19 +1853,39 @@
       <c r="Y25" s="1"/>
     </row>
     <row r="26" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
+      <c r="A26" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>70</v>
+      </c>
       <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
+      <c r="F26" s="1">
+        <v>2</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
-      <c r="J26" s="1"/>
-      <c r="K26" s="1"/>
+      <c r="I26" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="L26" s="1"/>
-      <c r="M26" s="1"/>
+      <c r="M26" s="1">
+        <v>10</v>
+      </c>
       <c r="N26" s="1"/>
       <c r="O26" s="1"/>
       <c r="P26" s="1"/>
@@ -1777,19 +1900,39 @@
       <c r="Y26" s="1"/>
     </row>
     <row r="27" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
+      <c r="A27" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>70</v>
+      </c>
       <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
+      <c r="F27" s="1">
+        <v>2</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="H27" s="1"/>
-      <c r="I27" s="1"/>
-      <c r="J27" s="1"/>
-      <c r="K27" s="1"/>
+      <c r="I27" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="L27" s="1"/>
-      <c r="M27" s="1"/>
+      <c r="M27" s="1">
+        <v>10</v>
+      </c>
       <c r="N27" s="1"/>
       <c r="O27" s="1"/>
       <c r="P27" s="1"/>
@@ -1804,19 +1947,39 @@
       <c r="Y27" s="1"/>
     </row>
     <row r="28" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
+      <c r="A28" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>70</v>
+      </c>
       <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
+      <c r="F28" s="1">
+        <v>1</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="H28" s="1"/>
-      <c r="I28" s="1"/>
-      <c r="J28" s="1"/>
-      <c r="K28" s="1"/>
+      <c r="I28" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="L28" s="1"/>
-      <c r="M28" s="1"/>
+      <c r="M28" s="1">
+        <v>10</v>
+      </c>
       <c r="N28" s="1"/>
       <c r="O28" s="1"/>
       <c r="P28" s="1"/>
@@ -1831,19 +1994,39 @@
       <c r="Y28" s="1"/>
     </row>
     <row r="29" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
+      <c r="A29" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>104</v>
+      </c>
       <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
+      <c r="F29" s="1">
+        <v>3</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="H29" s="1"/>
-      <c r="I29" s="1"/>
-      <c r="J29" s="1"/>
-      <c r="K29" s="1"/>
+      <c r="I29" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="L29" s="1"/>
-      <c r="M29" s="1"/>
+      <c r="M29" s="1">
+        <v>10</v>
+      </c>
       <c r="N29" s="1"/>
       <c r="O29" s="1"/>
       <c r="P29" s="1"/>
@@ -1858,19 +2041,39 @@
       <c r="Y29" s="1"/>
     </row>
     <row r="30" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
+      <c r="A30" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>108</v>
+      </c>
       <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
-      <c r="G30" s="1"/>
+      <c r="F30" s="1">
+        <v>3</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="H30" s="1"/>
-      <c r="I30" s="1"/>
-      <c r="J30" s="1"/>
-      <c r="K30" s="1"/>
+      <c r="I30" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K30" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="L30" s="1"/>
-      <c r="M30" s="1"/>
+      <c r="M30" s="1">
+        <v>10</v>
+      </c>
       <c r="N30" s="1"/>
       <c r="O30" s="1"/>
       <c r="P30" s="1"/>
@@ -1885,19 +2088,39 @@
       <c r="Y30" s="1"/>
     </row>
     <row r="31" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
+      <c r="A31" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>112</v>
+      </c>
       <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
+      <c r="F31" s="1">
+        <v>2</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="H31" s="1"/>
-      <c r="I31" s="1"/>
-      <c r="J31" s="1"/>
-      <c r="K31" s="1"/>
+      <c r="I31" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K31" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="L31" s="1"/>
-      <c r="M31" s="1"/>
+      <c r="M31" s="1">
+        <v>10</v>
+      </c>
       <c r="N31" s="1"/>
       <c r="O31" s="1"/>
       <c r="P31" s="1"/>
@@ -1912,19 +2135,39 @@
       <c r="Y31" s="1"/>
     </row>
     <row r="32" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
+      <c r="A32" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>116</v>
+      </c>
       <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
+      <c r="F32" s="1">
+        <v>1</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="H32" s="1"/>
-      <c r="I32" s="1"/>
-      <c r="J32" s="1"/>
-      <c r="K32" s="1"/>
+      <c r="I32" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K32" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="L32" s="1"/>
-      <c r="M32" s="1"/>
+      <c r="M32" s="1">
+        <v>10</v>
+      </c>
       <c r="N32" s="1"/>
       <c r="O32" s="1"/>
       <c r="P32" s="1"/>
@@ -1939,19 +2182,39 @@
       <c r="Y32" s="1"/>
     </row>
     <row r="33" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="1"/>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
+      <c r="A33" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>120</v>
+      </c>
       <c r="E33" s="1"/>
-      <c r="F33" s="1"/>
-      <c r="G33" s="1"/>
+      <c r="F33" s="1">
+        <v>1</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="H33" s="1"/>
-      <c r="I33" s="1"/>
-      <c r="J33" s="1"/>
-      <c r="K33" s="1"/>
+      <c r="I33" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K33" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="L33" s="1"/>
-      <c r="M33" s="1"/>
+      <c r="M33" s="1">
+        <v>10</v>
+      </c>
       <c r="N33" s="1"/>
       <c r="O33" s="1"/>
       <c r="P33" s="1"/>
@@ -1966,19 +2229,39 @@
       <c r="Y33" s="1"/>
     </row>
     <row r="34" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A34" s="1"/>
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
+      <c r="A34" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>118</v>
+      </c>
       <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
+      <c r="F34" s="1">
+        <v>3</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="H34" s="1"/>
-      <c r="I34" s="1"/>
-      <c r="J34" s="1"/>
-      <c r="K34" s="1"/>
+      <c r="I34" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J34" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K34" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="L34" s="1"/>
-      <c r="M34" s="1"/>
+      <c r="M34" s="1">
+        <v>10</v>
+      </c>
       <c r="N34" s="1"/>
       <c r="O34" s="1"/>
       <c r="P34" s="1"/>
@@ -1993,19 +2276,39 @@
       <c r="Y34" s="1"/>
     </row>
     <row r="35" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A35" s="1"/>
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
+      <c r="A35" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>112</v>
+      </c>
       <c r="E35" s="1"/>
-      <c r="F35" s="1"/>
-      <c r="G35" s="1"/>
+      <c r="F35" s="1">
+        <v>3</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="H35" s="1"/>
-      <c r="I35" s="1"/>
-      <c r="J35" s="1"/>
-      <c r="K35" s="1"/>
+      <c r="I35" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J35" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K35" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="L35" s="1"/>
-      <c r="M35" s="1"/>
+      <c r="M35" s="1">
+        <v>10</v>
+      </c>
       <c r="N35" s="1"/>
       <c r="O35" s="1"/>
       <c r="P35" s="1"/>

</xml_diff>